<commit_message>
added dependancie and small changes to documents
</commit_message>
<xml_diff>
--- a/Documents/CREDITORS ALLOWANCES JOURNAL TEMPLATE.xlsx
+++ b/Documents/CREDITORS ALLOWANCES JOURNAL TEMPLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydnicholson/Documents/GitHub/accounting-app/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7947E86C-98D1-794C-AA7B-460B680F2BE2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C50F981-D85A-B945-88E1-F50BD3FFD6E8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{998BA5AC-A104-FF4D-BE67-4CE905058659}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{998BA5AC-A104-FF4D-BE67-4CE905058659}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
     <t>Equipment</t>
   </si>
   <si>
-    <t>CREDITORS ALLOWANCES JOURNAL OF Big Gig for July 2016</t>
+    <t>CREDITORS ALLOWANCES JOURNAL OF</t>
   </si>
 </sst>
 </file>
@@ -823,7 +823,7 @@
   <dimension ref="B3:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H9" sqref="B9:H9"/>
+      <selection activeCell="B5" sqref="B5:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>